<commit_message>
Revert "Revert "Week 7""
This reverts commit 5e1053bd51ec7b2eea4179aaf1863a0c6b9e7474.
</commit_message>
<xml_diff>
--- a/Monthly_Reports/Monthly_Data/2021 Charts Month 1.xlsx
+++ b/Monthly_Reports/Monthly_Data/2021 Charts Month 1.xlsx
@@ -54,12 +54,12 @@
     <t>Don Diablo</t>
   </si>
   <si>
+    <t>KEVU</t>
+  </si>
+  <si>
     <t>Kaskade</t>
   </si>
   <si>
-    <t>KEVU</t>
-  </si>
-  <si>
     <t>Kirara Magic</t>
   </si>
   <si>
@@ -108,12 +108,12 @@
     <t>Matt Nash, Lucas Marx</t>
   </si>
   <si>
+    <t>Malarkey</t>
+  </si>
+  <si>
     <t>Polygon, Martin Jasper</t>
   </si>
   <si>
-    <t>Malarkey</t>
-  </si>
-  <si>
     <t>Lulleaux</t>
   </si>
   <si>
@@ -129,12 +129,12 @@
     <t>NUZB</t>
   </si>
   <si>
+    <t>Body Ocean</t>
+  </si>
+  <si>
     <t>Maurice Lessing</t>
   </si>
   <si>
-    <t>Body Ocean</t>
-  </si>
-  <si>
     <t>REGGIO, Rave Republic</t>
   </si>
   <si>
@@ -192,12 +192,12 @@
     <t>Into The Unknown</t>
   </si>
   <si>
+    <t>Melody</t>
+  </si>
+  <si>
     <t>Closer</t>
   </si>
   <si>
-    <t>Melody</t>
-  </si>
-  <si>
     <t>Wraith</t>
   </si>
   <si>
@@ -246,12 +246,12 @@
     <t>Midnight</t>
   </si>
   <si>
+    <t>Shackles (Praise You)</t>
+  </si>
+  <si>
     <t>Coming Home</t>
   </si>
   <si>
-    <t>Shackles (Praise You)</t>
-  </si>
-  <si>
     <t>Even If You Don't</t>
   </si>
   <si>
@@ -267,12 +267,12 @@
     <t>Nighttime</t>
   </si>
   <si>
+    <t>Once The Music</t>
+  </si>
+  <si>
     <t>Never Let You Go</t>
   </si>
   <si>
-    <t>Once The Music</t>
-  </si>
-  <si>
     <t>Legacy</t>
   </si>
   <si>
@@ -330,10 +330,10 @@
     <t>HEXAGON</t>
   </si>
   <si>
+    <t>Maxximize Records, Spinnin' Records</t>
+  </si>
+  <si>
     <t>Monstercat</t>
-  </si>
-  <si>
-    <t>Maxximize Records, Spinnin' Records</t>
   </si>
   <si>
     <t>NONE</t>
@@ -920,7 +920,7 @@
         <v>97</v>
       </c>
       <c r="D2">
-        <v>2443226</v>
+        <v>2631252</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -934,7 +934,7 @@
         <v>98</v>
       </c>
       <c r="D3">
-        <v>1215313</v>
+        <v>1296610</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -948,7 +948,7 @@
         <v>99</v>
       </c>
       <c r="D4">
-        <v>1197598</v>
+        <v>1220449</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -962,7 +962,7 @@
         <v>99</v>
       </c>
       <c r="D5">
-        <v>936064</v>
+        <v>955772</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -976,7 +976,7 @@
         <v>100</v>
       </c>
       <c r="D6">
-        <v>818990</v>
+        <v>830548</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -990,7 +990,7 @@
         <v>101</v>
       </c>
       <c r="D7">
-        <v>673909</v>
+        <v>695603</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -1004,7 +1004,7 @@
         <v>102</v>
       </c>
       <c r="D8">
-        <v>385867</v>
+        <v>473116</v>
       </c>
     </row>
     <row r="9" spans="1:4">
@@ -1018,7 +1018,7 @@
         <v>103</v>
       </c>
       <c r="D9">
-        <v>365179</v>
+        <v>416185</v>
       </c>
     </row>
     <row r="10" spans="1:4">
@@ -1032,7 +1032,7 @@
         <v>104</v>
       </c>
       <c r="D10">
-        <v>318074</v>
+        <v>364686</v>
       </c>
     </row>
     <row r="11" spans="1:4">
@@ -1046,7 +1046,7 @@
         <v>105</v>
       </c>
       <c r="D11">
-        <v>311782</v>
+        <v>336188</v>
       </c>
     </row>
     <row r="12" spans="1:4">
@@ -1060,7 +1060,7 @@
         <v>106</v>
       </c>
       <c r="D12">
-        <v>284844</v>
+        <v>303531</v>
       </c>
     </row>
     <row r="13" spans="1:4">
@@ -1074,7 +1074,7 @@
         <v>107</v>
       </c>
       <c r="D13">
-        <v>218096</v>
+        <v>227242</v>
       </c>
     </row>
     <row r="14" spans="1:4">
@@ -1085,10 +1085,10 @@
         <v>62</v>
       </c>
       <c r="C14" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="D14">
-        <v>176822</v>
+        <v>187158</v>
       </c>
     </row>
     <row r="15" spans="1:4">
@@ -1102,7 +1102,7 @@
         <v>108</v>
       </c>
       <c r="D15">
-        <v>140727</v>
+        <v>150182</v>
       </c>
     </row>
     <row r="16" spans="1:4">
@@ -1116,7 +1116,7 @@
         <v>107</v>
       </c>
       <c r="D16">
-        <v>124757</v>
+        <v>129542</v>
       </c>
     </row>
     <row r="17" spans="1:4">
@@ -1127,10 +1127,10 @@
         <v>65</v>
       </c>
       <c r="C17" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="D17">
-        <v>124436</v>
+        <v>129229</v>
       </c>
     </row>
     <row r="18" spans="1:4">
@@ -1144,7 +1144,7 @@
         <v>104</v>
       </c>
       <c r="D18">
-        <v>115103</v>
+        <v>119609</v>
       </c>
     </row>
     <row r="19" spans="1:4">
@@ -1158,7 +1158,7 @@
         <v>104</v>
       </c>
       <c r="D19">
-        <v>110071</v>
+        <v>116440</v>
       </c>
     </row>
     <row r="20" spans="1:4">
@@ -1169,10 +1169,10 @@
         <v>68</v>
       </c>
       <c r="C20" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="D20">
-        <v>107203</v>
+        <v>114821</v>
       </c>
     </row>
     <row r="21" spans="1:4">
@@ -1186,7 +1186,7 @@
         <v>107</v>
       </c>
       <c r="D21">
-        <v>79132</v>
+        <v>81963</v>
       </c>
     </row>
     <row r="22" spans="1:4">
@@ -1200,7 +1200,7 @@
         <v>109</v>
       </c>
       <c r="D22">
-        <v>77822</v>
+        <v>78952</v>
       </c>
     </row>
     <row r="23" spans="1:4">
@@ -1214,7 +1214,7 @@
         <v>110</v>
       </c>
       <c r="D23">
-        <v>68416</v>
+        <v>71826</v>
       </c>
     </row>
     <row r="24" spans="1:4">
@@ -1228,7 +1228,7 @@
         <v>104</v>
       </c>
       <c r="D24">
-        <v>63380</v>
+        <v>66907</v>
       </c>
     </row>
     <row r="25" spans="1:4">
@@ -1242,7 +1242,7 @@
         <v>107</v>
       </c>
       <c r="D25">
-        <v>59890</v>
+        <v>61794</v>
       </c>
     </row>
     <row r="26" spans="1:4">
@@ -1253,10 +1253,10 @@
         <v>74</v>
       </c>
       <c r="C26" t="s">
-        <v>111</v>
+        <v>101</v>
       </c>
       <c r="D26">
-        <v>49652</v>
+        <v>53132</v>
       </c>
     </row>
     <row r="27" spans="1:4">
@@ -1267,10 +1267,10 @@
         <v>75</v>
       </c>
       <c r="C27" t="s">
-        <v>101</v>
+        <v>111</v>
       </c>
       <c r="D27">
-        <v>48234</v>
+        <v>52061</v>
       </c>
     </row>
     <row r="28" spans="1:4">
@@ -1284,7 +1284,7 @@
         <v>101</v>
       </c>
       <c r="D28">
-        <v>44523</v>
+        <v>47650</v>
       </c>
     </row>
     <row r="29" spans="1:4">
@@ -1298,7 +1298,7 @@
         <v>101</v>
       </c>
       <c r="D29">
-        <v>41511</v>
+        <v>42427</v>
       </c>
     </row>
     <row r="30" spans="1:4">
@@ -1312,7 +1312,7 @@
         <v>110</v>
       </c>
       <c r="D30">
-        <v>38208</v>
+        <v>40015</v>
       </c>
     </row>
     <row r="31" spans="1:4">
@@ -1326,7 +1326,7 @@
         <v>110</v>
       </c>
       <c r="D31">
-        <v>33137</v>
+        <v>34164</v>
       </c>
     </row>
     <row r="32" spans="1:4">
@@ -1340,7 +1340,7 @@
         <v>107</v>
       </c>
       <c r="D32">
-        <v>30074</v>
+        <v>31171</v>
       </c>
     </row>
     <row r="33" spans="1:4">
@@ -1351,10 +1351,10 @@
         <v>81</v>
       </c>
       <c r="C33" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D33">
-        <v>29107</v>
+        <v>30210</v>
       </c>
     </row>
     <row r="34" spans="1:4">
@@ -1365,10 +1365,10 @@
         <v>82</v>
       </c>
       <c r="C34" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="D34">
-        <v>28682</v>
+        <v>29360</v>
       </c>
     </row>
     <row r="35" spans="1:4">
@@ -1382,7 +1382,7 @@
         <v>110</v>
       </c>
       <c r="D35">
-        <v>21522</v>
+        <v>22164</v>
       </c>
     </row>
     <row r="36" spans="1:4">
@@ -1396,7 +1396,7 @@
         <v>107</v>
       </c>
       <c r="D36">
-        <v>17297</v>
+        <v>17511</v>
       </c>
     </row>
     <row r="37" spans="1:4">
@@ -1410,7 +1410,7 @@
         <v>110</v>
       </c>
       <c r="D37">
-        <v>10947</v>
+        <v>11191</v>
       </c>
     </row>
     <row r="38" spans="1:4">
@@ -1424,7 +1424,7 @@
         <v>112</v>
       </c>
       <c r="D38">
-        <v>8549</v>
+        <v>8751</v>
       </c>
     </row>
     <row r="39" spans="1:4">
@@ -1438,7 +1438,7 @@
         <v>113</v>
       </c>
       <c r="D39">
-        <v>7753</v>
+        <v>7950</v>
       </c>
     </row>
     <row r="40" spans="1:4">
@@ -1452,7 +1452,7 @@
         <v>114</v>
       </c>
       <c r="D40">
-        <v>6358</v>
+        <v>6530</v>
       </c>
     </row>
     <row r="41" spans="1:4">
@@ -1466,7 +1466,7 @@
         <v>115</v>
       </c>
       <c r="D41">
-        <v>5923</v>
+        <v>6045</v>
       </c>
     </row>
     <row r="42" spans="1:4">
@@ -1480,7 +1480,7 @@
         <v>116</v>
       </c>
       <c r="D42">
-        <v>4861</v>
+        <v>5425</v>
       </c>
     </row>
     <row r="43" spans="1:4">
@@ -1494,7 +1494,7 @@
         <v>117</v>
       </c>
       <c r="D43">
-        <v>4140</v>
+        <v>4216</v>
       </c>
     </row>
     <row r="44" spans="1:4">
@@ -1508,7 +1508,7 @@
         <v>117</v>
       </c>
       <c r="D44">
-        <v>4003</v>
+        <v>4094</v>
       </c>
     </row>
     <row r="45" spans="1:4">
@@ -1522,7 +1522,7 @@
         <v>113</v>
       </c>
       <c r="D45">
-        <v>2448</v>
+        <v>2538</v>
       </c>
     </row>
     <row r="46" spans="1:4">
@@ -1536,7 +1536,7 @@
         <v>118</v>
       </c>
       <c r="D46">
-        <v>1876</v>
+        <v>2050</v>
       </c>
     </row>
     <row r="47" spans="1:4">
@@ -1550,7 +1550,7 @@
         <v>119</v>
       </c>
       <c r="D47">
-        <v>1080</v>
+        <v>1166</v>
       </c>
     </row>
     <row r="48" spans="1:4">
@@ -1599,10 +1599,10 @@
     </row>
     <row r="2" spans="1:5">
       <c r="A2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C2" t="s">
         <v>101</v>
@@ -1611,58 +1611,58 @@
         <v>100</v>
       </c>
       <c r="E2">
-        <v>119</v>
+        <v>120</v>
       </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C3" t="s">
         <v>107</v>
       </c>
       <c r="D3">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="E3">
-        <v>97</v>
+        <v>100</v>
       </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" t="s">
-        <v>23</v>
+        <v>5</v>
       </c>
       <c r="B4" t="s">
-        <v>69</v>
+        <v>52</v>
       </c>
       <c r="C4" t="s">
-        <v>107</v>
+        <v>98</v>
       </c>
       <c r="D4">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="E4">
-        <v>99</v>
+        <v>108</v>
       </c>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" t="s">
-        <v>5</v>
+        <v>23</v>
       </c>
       <c r="B5" t="s">
-        <v>52</v>
+        <v>69</v>
       </c>
       <c r="C5" t="s">
-        <v>98</v>
+        <v>107</v>
       </c>
       <c r="D5">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="E5">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -1679,7 +1679,7 @@
         <v>58</v>
       </c>
       <c r="E6">
-        <v>64</v>
+        <v>65</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -1693,10 +1693,10 @@
         <v>101</v>
       </c>
       <c r="D7">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="E7">
-        <v>57</v>
+        <v>59</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -1710,10 +1710,10 @@
         <v>107</v>
       </c>
       <c r="D8">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="E8">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -1727,18 +1727,18 @@
         <v>107</v>
       </c>
       <c r="D9">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="E9">
-        <v>45</v>
+        <v>48</v>
       </c>
     </row>
     <row r="10" spans="1:5">
       <c r="A10" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B10" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="C10" t="s">
         <v>108</v>
@@ -1781,7 +1781,7 @@
         <v>32</v>
       </c>
       <c r="E12">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="13" spans="1:5">
@@ -1820,36 +1820,36 @@
     </row>
     <row r="15" spans="1:5">
       <c r="A15" t="s">
-        <v>8</v>
+        <v>41</v>
       </c>
       <c r="B15" t="s">
-        <v>54</v>
+        <v>87</v>
       </c>
       <c r="C15" t="s">
-        <v>100</v>
+        <v>113</v>
       </c>
       <c r="D15">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="E15">
-        <v>41</v>
+        <v>28</v>
       </c>
     </row>
     <row r="16" spans="1:5">
       <c r="A16" t="s">
-        <v>41</v>
+        <v>8</v>
       </c>
       <c r="B16" t="s">
-        <v>87</v>
+        <v>54</v>
       </c>
       <c r="C16" t="s">
-        <v>113</v>
+        <v>100</v>
       </c>
       <c r="D16">
         <v>25</v>
       </c>
       <c r="E16">
-        <v>26</v>
+        <v>42</v>
       </c>
     </row>
     <row r="17" spans="1:5">
@@ -1956,19 +1956,19 @@
     </row>
     <row r="23" spans="1:5">
       <c r="A23" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B23" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C23" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="D23">
         <v>12</v>
       </c>
       <c r="E23">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="24" spans="1:5">
@@ -1982,10 +1982,10 @@
         <v>110</v>
       </c>
       <c r="D24">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E24">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="25" spans="1:5">
@@ -2007,13 +2007,13 @@
     </row>
     <row r="26" spans="1:5">
       <c r="A26" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B26" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C26" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D26">
         <v>8</v>
@@ -2030,7 +2030,7 @@
         <v>65</v>
       </c>
       <c r="C27" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="D27">
         <v>7</v>
@@ -2098,7 +2098,7 @@
         <v>62</v>
       </c>
       <c r="C31" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="D31">
         <v>6</v>
@@ -2143,10 +2143,10 @@
     </row>
     <row r="34" spans="1:5">
       <c r="A34" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B34" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="C34" t="s">
         <v>111</v>
@@ -2166,7 +2166,7 @@
         <v>68</v>
       </c>
       <c r="C35" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="D35">
         <v>1</v>
@@ -2434,7 +2434,7 @@
         <v>97</v>
       </c>
       <c r="D2">
-        <v>138148</v>
+        <v>147082</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -2445,10 +2445,10 @@
         <v>65</v>
       </c>
       <c r="C3" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="D3">
-        <v>96907</v>
+        <v>99991</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -2462,21 +2462,21 @@
         <v>100</v>
       </c>
       <c r="D4">
-        <v>88196</v>
+        <v>94648</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B5" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C5" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="D5">
-        <v>84178</v>
+        <v>89181</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -2487,10 +2487,10 @@
         <v>62</v>
       </c>
       <c r="C6" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="D6">
-        <v>66583</v>
+        <v>69549</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -2501,10 +2501,10 @@
         <v>68</v>
       </c>
       <c r="C7" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="D7">
-        <v>58202</v>
+        <v>61960</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -2518,21 +2518,21 @@
         <v>98</v>
       </c>
       <c r="D8">
-        <v>45584</v>
+        <v>49556</v>
       </c>
     </row>
     <row r="9" spans="1:4">
       <c r="A9" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="B9" t="s">
-        <v>53</v>
+        <v>59</v>
       </c>
       <c r="C9" t="s">
-        <v>99</v>
+        <v>105</v>
       </c>
       <c r="D9">
-        <v>39031</v>
+        <v>36609</v>
       </c>
     </row>
     <row r="10" spans="1:4">
@@ -2546,105 +2546,105 @@
         <v>99</v>
       </c>
       <c r="D10">
-        <v>33883</v>
+        <v>35234</v>
       </c>
     </row>
     <row r="11" spans="1:4">
       <c r="A11" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B11" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="C11" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="D11">
-        <v>33634</v>
+        <v>29971</v>
       </c>
     </row>
     <row r="12" spans="1:4">
       <c r="A12" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B12" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C12" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D12">
-        <v>28389</v>
+        <v>22750</v>
       </c>
     </row>
     <row r="13" spans="1:4">
       <c r="A13" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="B13" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="C13" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="D13">
-        <v>21409</v>
+        <v>22157</v>
       </c>
     </row>
     <row r="14" spans="1:4">
       <c r="A14" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C14" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="D14">
-        <v>21192</v>
+        <v>20881</v>
       </c>
     </row>
     <row r="15" spans="1:4">
       <c r="A15" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="B15" t="s">
-        <v>58</v>
+        <v>64</v>
       </c>
       <c r="C15" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="D15">
-        <v>20019</v>
+        <v>20178</v>
       </c>
     </row>
     <row r="16" spans="1:4">
       <c r="A16" t="s">
-        <v>18</v>
+        <v>30</v>
       </c>
       <c r="B16" t="s">
-        <v>64</v>
+        <v>76</v>
       </c>
       <c r="C16" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="D16">
-        <v>19051</v>
+        <v>18836</v>
       </c>
     </row>
     <row r="17" spans="1:4">
       <c r="A17" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B17" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C17" t="s">
         <v>101</v>
       </c>
       <c r="D17">
-        <v>17680</v>
+        <v>17374</v>
       </c>
     </row>
     <row r="18" spans="1:4">
@@ -2658,382 +2658,382 @@
         <v>110</v>
       </c>
       <c r="D18">
-        <v>16254</v>
+        <v>17079</v>
       </c>
     </row>
     <row r="19" spans="1:4">
       <c r="A19" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B19" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="C19" t="s">
         <v>101</v>
       </c>
       <c r="D19">
-        <v>16246</v>
+        <v>16918</v>
       </c>
     </row>
     <row r="20" spans="1:4">
       <c r="A20" t="s">
-        <v>31</v>
+        <v>50</v>
       </c>
       <c r="B20" t="s">
-        <v>77</v>
+        <v>96</v>
       </c>
       <c r="C20" t="s">
-        <v>101</v>
+        <v>120</v>
       </c>
       <c r="D20">
-        <v>16165</v>
+        <v>16317</v>
       </c>
     </row>
     <row r="21" spans="1:4">
       <c r="A21" t="s">
-        <v>50</v>
+        <v>34</v>
       </c>
       <c r="B21" t="s">
-        <v>96</v>
+        <v>80</v>
       </c>
       <c r="C21" t="s">
-        <v>120</v>
+        <v>107</v>
       </c>
       <c r="D21">
-        <v>15567</v>
+        <v>16197</v>
       </c>
     </row>
     <row r="22" spans="1:4">
       <c r="A22" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="B22" t="s">
-        <v>80</v>
+        <v>72</v>
       </c>
       <c r="C22" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="D22">
-        <v>14908</v>
+        <v>14922</v>
       </c>
     </row>
     <row r="23" spans="1:4">
       <c r="A23" t="s">
-        <v>26</v>
+        <v>43</v>
       </c>
       <c r="B23" t="s">
-        <v>72</v>
+        <v>89</v>
       </c>
       <c r="C23" t="s">
-        <v>104</v>
+        <v>115</v>
       </c>
       <c r="D23">
-        <v>14089</v>
+        <v>13578</v>
       </c>
     </row>
     <row r="24" spans="1:4">
       <c r="A24" t="s">
-        <v>43</v>
+        <v>27</v>
       </c>
       <c r="B24" t="s">
-        <v>89</v>
+        <v>73</v>
       </c>
       <c r="C24" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
       <c r="D24">
-        <v>13100</v>
+        <v>13578</v>
       </c>
     </row>
     <row r="25" spans="1:4">
       <c r="A25" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B25" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C25" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
       <c r="D25">
-        <v>12437</v>
+        <v>13061</v>
       </c>
     </row>
     <row r="26" spans="1:4">
       <c r="A26" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B26" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C26" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D26">
-        <v>12187</v>
+        <v>11527</v>
       </c>
     </row>
     <row r="27" spans="1:4">
       <c r="A27" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="B27" t="s">
-        <v>70</v>
+        <v>75</v>
       </c>
       <c r="C27" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="D27">
-        <v>10989</v>
+        <v>10788</v>
       </c>
     </row>
     <row r="28" spans="1:4">
       <c r="A28" t="s">
-        <v>28</v>
+        <v>17</v>
       </c>
       <c r="B28" t="s">
-        <v>74</v>
+        <v>63</v>
       </c>
       <c r="C28" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="D28">
-        <v>10335</v>
+        <v>10398</v>
       </c>
     </row>
     <row r="29" spans="1:4">
       <c r="A29" t="s">
-        <v>17</v>
+        <v>36</v>
       </c>
       <c r="B29" t="s">
-        <v>63</v>
+        <v>82</v>
       </c>
       <c r="C29" t="s">
         <v>108</v>
       </c>
       <c r="D29">
-        <v>10032</v>
+        <v>9833</v>
       </c>
     </row>
     <row r="30" spans="1:4">
       <c r="A30" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="B30" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="C30" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="D30">
-        <v>9391</v>
+        <v>8691</v>
       </c>
     </row>
     <row r="31" spans="1:4">
       <c r="A31" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="B31" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="C31" t="s">
         <v>107</v>
       </c>
       <c r="D31">
-        <v>9013</v>
+        <v>8528</v>
       </c>
     </row>
     <row r="32" spans="1:4">
       <c r="A32" t="s">
-        <v>32</v>
+        <v>47</v>
       </c>
       <c r="B32" t="s">
-        <v>78</v>
+        <v>93</v>
       </c>
       <c r="C32" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
       <c r="D32">
-        <v>8297</v>
+        <v>8088</v>
       </c>
     </row>
     <row r="33" spans="1:4">
       <c r="A33" t="s">
-        <v>36</v>
+        <v>44</v>
       </c>
       <c r="B33" t="s">
-        <v>82</v>
+        <v>90</v>
       </c>
       <c r="C33" t="s">
-        <v>107</v>
+        <v>116</v>
       </c>
       <c r="D33">
-        <v>7750</v>
+        <v>7162</v>
       </c>
     </row>
     <row r="34" spans="1:4">
       <c r="A34" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="B34" t="s">
-        <v>93</v>
+        <v>86</v>
       </c>
       <c r="C34" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D34">
-        <v>7591</v>
+        <v>7056</v>
       </c>
     </row>
     <row r="35" spans="1:4">
       <c r="A35" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="B35" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="C35" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="D35">
-        <v>6876</v>
+        <v>6899</v>
       </c>
     </row>
     <row r="36" spans="1:4">
       <c r="A36" t="s">
-        <v>33</v>
+        <v>49</v>
       </c>
       <c r="B36" t="s">
-        <v>79</v>
+        <v>95</v>
       </c>
       <c r="C36" t="s">
-        <v>110</v>
+        <v>119</v>
       </c>
       <c r="D36">
-        <v>6627</v>
+        <v>5109</v>
       </c>
     </row>
     <row r="37" spans="1:4">
       <c r="A37" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="B37" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="C37" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="D37">
-        <v>6334</v>
+        <v>4157</v>
       </c>
     </row>
     <row r="38" spans="1:4">
       <c r="A38" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="B38" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="C38" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="D38">
-        <v>4933</v>
+        <v>2165</v>
       </c>
     </row>
     <row r="39" spans="1:4">
       <c r="A39" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="B39" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="C39" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
       <c r="D39">
-        <v>4045</v>
+        <v>1502</v>
       </c>
     </row>
     <row r="40" spans="1:4">
       <c r="A40" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B40" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C40" t="s">
         <v>117</v>
       </c>
       <c r="D40">
-        <v>2086</v>
+        <v>1472</v>
       </c>
     </row>
     <row r="41" spans="1:4">
       <c r="A41" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B41" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="C41" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="D41">
-        <v>1457</v>
+        <v>1376</v>
       </c>
     </row>
     <row r="42" spans="1:4">
       <c r="A42" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="B42" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="C42" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="D42">
-        <v>1419</v>
+        <v>503</v>
       </c>
     </row>
     <row r="43" spans="1:4">
       <c r="A43" t="s">
-        <v>42</v>
+        <v>7</v>
       </c>
       <c r="B43" t="s">
-        <v>88</v>
+        <v>53</v>
       </c>
       <c r="C43" t="s">
-        <v>114</v>
+        <v>99</v>
       </c>
       <c r="D43">
-        <v>1274</v>
+        <v>0</v>
       </c>
     </row>
     <row r="44" spans="1:4">
       <c r="A44" t="s">
-        <v>48</v>
+        <v>21</v>
       </c>
       <c r="B44" t="s">
-        <v>94</v>
+        <v>67</v>
       </c>
       <c r="C44" t="s">
-        <v>118</v>
+        <v>104</v>
       </c>
       <c r="D44">
-        <v>459</v>
+        <v>0</v>
       </c>
     </row>
     <row r="45" spans="1:4">
       <c r="A45" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B45" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="C45" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="D45">
         <v>0</v>
@@ -3041,13 +3041,13 @@
     </row>
     <row r="46" spans="1:4">
       <c r="A46" t="s">
-        <v>23</v>
+        <v>9</v>
       </c>
       <c r="B46" t="s">
-        <v>69</v>
+        <v>55</v>
       </c>
       <c r="C46" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="D46">
         <v>0</v>
@@ -3055,13 +3055,13 @@
     </row>
     <row r="47" spans="1:4">
       <c r="A47" t="s">
-        <v>9</v>
+        <v>38</v>
       </c>
       <c r="B47" t="s">
-        <v>55</v>
+        <v>84</v>
       </c>
       <c r="C47" t="s">
-        <v>101</v>
+        <v>107</v>
       </c>
       <c r="D47">
         <v>0</v>
@@ -3107,7 +3107,7 @@
         <v>4</v>
       </c>
       <c r="B2">
-        <v>2443226</v>
+        <v>2631252</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -3115,7 +3115,7 @@
         <v>5</v>
       </c>
       <c r="B3">
-        <v>1215313</v>
+        <v>1296610</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -3123,7 +3123,7 @@
         <v>124</v>
       </c>
       <c r="B4">
-        <v>1197598</v>
+        <v>1220449</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -3131,7 +3131,7 @@
         <v>125</v>
       </c>
       <c r="B5">
-        <v>1197598</v>
+        <v>1220449</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -3139,7 +3139,7 @@
         <v>7</v>
       </c>
       <c r="B6">
-        <v>936064</v>
+        <v>955772</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -3147,7 +3147,7 @@
         <v>126</v>
       </c>
       <c r="B7">
-        <v>818990</v>
+        <v>830548</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -3155,7 +3155,7 @@
         <v>127</v>
       </c>
       <c r="B8">
-        <v>818990</v>
+        <v>830548</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -3163,7 +3163,7 @@
         <v>9</v>
       </c>
       <c r="B9">
-        <v>673909</v>
+        <v>695603</v>
       </c>
     </row>
     <row r="10" spans="1:2">
@@ -3171,7 +3171,7 @@
         <v>10</v>
       </c>
       <c r="B10">
-        <v>385867</v>
+        <v>473116</v>
       </c>
     </row>
     <row r="11" spans="1:2">
@@ -3179,7 +3179,7 @@
         <v>11</v>
       </c>
       <c r="B11">
-        <v>365179</v>
+        <v>416185</v>
       </c>
     </row>
     <row r="12" spans="1:2">
@@ -3187,7 +3187,7 @@
         <v>12</v>
       </c>
       <c r="B12">
-        <v>318074</v>
+        <v>364686</v>
       </c>
     </row>
     <row r="13" spans="1:2">
@@ -3195,7 +3195,7 @@
         <v>13</v>
       </c>
       <c r="B13">
-        <v>311782</v>
+        <v>336188</v>
       </c>
     </row>
     <row r="14" spans="1:2">
@@ -3203,7 +3203,7 @@
         <v>14</v>
       </c>
       <c r="B14">
-        <v>284844</v>
+        <v>303531</v>
       </c>
     </row>
     <row r="15" spans="1:2">
@@ -3211,7 +3211,7 @@
         <v>15</v>
       </c>
       <c r="B15">
-        <v>218096</v>
+        <v>227242</v>
       </c>
     </row>
     <row r="16" spans="1:2">
@@ -3219,7 +3219,7 @@
         <v>16</v>
       </c>
       <c r="B16">
-        <v>176822</v>
+        <v>187158</v>
       </c>
     </row>
     <row r="17" spans="1:2">
@@ -3227,7 +3227,7 @@
         <v>17</v>
       </c>
       <c r="B17">
-        <v>140727</v>
+        <v>150182</v>
       </c>
     </row>
     <row r="18" spans="1:2">
@@ -3235,7 +3235,7 @@
         <v>18</v>
       </c>
       <c r="B18">
-        <v>124757</v>
+        <v>129542</v>
       </c>
     </row>
     <row r="19" spans="1:2">
@@ -3243,7 +3243,7 @@
         <v>128</v>
       </c>
       <c r="B19">
-        <v>124436</v>
+        <v>129229</v>
       </c>
     </row>
     <row r="20" spans="1:2">
@@ -3251,7 +3251,7 @@
         <v>129</v>
       </c>
       <c r="B20">
-        <v>124436</v>
+        <v>129229</v>
       </c>
     </row>
     <row r="21" spans="1:2">
@@ -3259,7 +3259,7 @@
         <v>20</v>
       </c>
       <c r="B21">
-        <v>115103</v>
+        <v>119609</v>
       </c>
     </row>
     <row r="22" spans="1:2">
@@ -3267,7 +3267,7 @@
         <v>21</v>
       </c>
       <c r="B22">
-        <v>110071</v>
+        <v>116440</v>
       </c>
     </row>
     <row r="23" spans="1:2">
@@ -3275,7 +3275,7 @@
         <v>22</v>
       </c>
       <c r="B23">
-        <v>107203</v>
+        <v>114821</v>
       </c>
     </row>
     <row r="24" spans="1:2">
@@ -3283,7 +3283,7 @@
         <v>23</v>
       </c>
       <c r="B24">
-        <v>79132</v>
+        <v>81963</v>
       </c>
     </row>
     <row r="25" spans="1:2">
@@ -3291,7 +3291,7 @@
         <v>24</v>
       </c>
       <c r="B25">
-        <v>77822</v>
+        <v>78952</v>
       </c>
     </row>
     <row r="26" spans="1:2">
@@ -3299,7 +3299,7 @@
         <v>130</v>
       </c>
       <c r="B26">
-        <v>68416</v>
+        <v>71826</v>
       </c>
     </row>
     <row r="27" spans="1:2">
@@ -3307,7 +3307,7 @@
         <v>131</v>
       </c>
       <c r="B27">
-        <v>68416</v>
+        <v>71826</v>
       </c>
     </row>
     <row r="28" spans="1:2">
@@ -3315,7 +3315,7 @@
         <v>26</v>
       </c>
       <c r="B28">
-        <v>63380</v>
+        <v>66907</v>
       </c>
     </row>
     <row r="29" spans="1:2">
@@ -3323,7 +3323,7 @@
         <v>132</v>
       </c>
       <c r="B29">
-        <v>59890</v>
+        <v>61794</v>
       </c>
     </row>
     <row r="30" spans="1:2">
@@ -3331,31 +3331,31 @@
         <v>133</v>
       </c>
       <c r="B30">
-        <v>59890</v>
+        <v>61794</v>
       </c>
     </row>
     <row r="31" spans="1:2">
       <c r="A31" s="1" t="s">
-        <v>134</v>
+        <v>28</v>
       </c>
       <c r="B31">
-        <v>49652</v>
+        <v>53132</v>
       </c>
     </row>
     <row r="32" spans="1:2">
       <c r="A32" s="1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B32">
-        <v>49652</v>
+        <v>52061</v>
       </c>
     </row>
     <row r="33" spans="1:2">
       <c r="A33" s="1" t="s">
-        <v>29</v>
+        <v>135</v>
       </c>
       <c r="B33">
-        <v>48234</v>
+        <v>52061</v>
       </c>
     </row>
     <row r="34" spans="1:2">
@@ -3363,7 +3363,7 @@
         <v>30</v>
       </c>
       <c r="B34">
-        <v>44523</v>
+        <v>47650</v>
       </c>
     </row>
     <row r="35" spans="1:2">
@@ -3371,7 +3371,7 @@
         <v>31</v>
       </c>
       <c r="B35">
-        <v>41511</v>
+        <v>42427</v>
       </c>
     </row>
     <row r="36" spans="1:2">
@@ -3379,7 +3379,7 @@
         <v>136</v>
       </c>
       <c r="B36">
-        <v>38208</v>
+        <v>40015</v>
       </c>
     </row>
     <row r="37" spans="1:2">
@@ -3387,7 +3387,7 @@
         <v>137</v>
       </c>
       <c r="B37">
-        <v>38208</v>
+        <v>40015</v>
       </c>
     </row>
     <row r="38" spans="1:2">
@@ -3395,7 +3395,7 @@
         <v>138</v>
       </c>
       <c r="B38">
-        <v>33137</v>
+        <v>34164</v>
       </c>
     </row>
     <row r="39" spans="1:2">
@@ -3403,7 +3403,7 @@
         <v>139</v>
       </c>
       <c r="B39">
-        <v>33137</v>
+        <v>34164</v>
       </c>
     </row>
     <row r="40" spans="1:2">
@@ -3411,7 +3411,7 @@
         <v>140</v>
       </c>
       <c r="B40">
-        <v>33137</v>
+        <v>34164</v>
       </c>
     </row>
     <row r="41" spans="1:2">
@@ -3419,7 +3419,7 @@
         <v>34</v>
       </c>
       <c r="B41">
-        <v>30074</v>
+        <v>31171</v>
       </c>
     </row>
     <row r="42" spans="1:2">
@@ -3427,7 +3427,7 @@
         <v>35</v>
       </c>
       <c r="B42">
-        <v>29107</v>
+        <v>30210</v>
       </c>
     </row>
     <row r="43" spans="1:2">
@@ -3435,7 +3435,7 @@
         <v>36</v>
       </c>
       <c r="B43">
-        <v>28682</v>
+        <v>29360</v>
       </c>
     </row>
     <row r="44" spans="1:2">
@@ -3443,7 +3443,7 @@
         <v>141</v>
       </c>
       <c r="B44">
-        <v>21522</v>
+        <v>22164</v>
       </c>
     </row>
     <row r="45" spans="1:2">
@@ -3451,7 +3451,7 @@
         <v>142</v>
       </c>
       <c r="B45">
-        <v>21522</v>
+        <v>22164</v>
       </c>
     </row>
     <row r="46" spans="1:2">
@@ -3459,7 +3459,7 @@
         <v>143</v>
       </c>
       <c r="B46">
-        <v>17297</v>
+        <v>17511</v>
       </c>
     </row>
     <row r="47" spans="1:2">
@@ -3467,7 +3467,7 @@
         <v>144</v>
       </c>
       <c r="B47">
-        <v>17297</v>
+        <v>17511</v>
       </c>
     </row>
     <row r="48" spans="1:2">
@@ -3475,7 +3475,7 @@
         <v>145</v>
       </c>
       <c r="B48">
-        <v>10947</v>
+        <v>11191</v>
       </c>
     </row>
     <row r="49" spans="1:2">
@@ -3483,7 +3483,7 @@
         <v>146</v>
       </c>
       <c r="B49">
-        <v>10947</v>
+        <v>11191</v>
       </c>
     </row>
     <row r="50" spans="1:2">
@@ -3491,7 +3491,7 @@
         <v>147</v>
       </c>
       <c r="B50">
-        <v>10947</v>
+        <v>11191</v>
       </c>
     </row>
     <row r="51" spans="1:2">
@@ -3499,7 +3499,7 @@
         <v>40</v>
       </c>
       <c r="B51">
-        <v>8549</v>
+        <v>8751</v>
       </c>
     </row>
     <row r="52" spans="1:2">
@@ -3507,7 +3507,7 @@
         <v>148</v>
       </c>
       <c r="B52">
-        <v>7753</v>
+        <v>7950</v>
       </c>
     </row>
     <row r="53" spans="1:2">
@@ -3515,7 +3515,7 @@
         <v>149</v>
       </c>
       <c r="B53">
-        <v>7753</v>
+        <v>7950</v>
       </c>
     </row>
     <row r="54" spans="1:2">
@@ -3523,7 +3523,7 @@
         <v>42</v>
       </c>
       <c r="B54">
-        <v>6358</v>
+        <v>6530</v>
       </c>
     </row>
     <row r="55" spans="1:2">
@@ -3531,7 +3531,7 @@
         <v>43</v>
       </c>
       <c r="B55">
-        <v>5923</v>
+        <v>6045</v>
       </c>
     </row>
     <row r="56" spans="1:2">
@@ -3539,7 +3539,7 @@
         <v>150</v>
       </c>
       <c r="B56">
-        <v>4861</v>
+        <v>5425</v>
       </c>
     </row>
     <row r="57" spans="1:2">
@@ -3547,7 +3547,7 @@
         <v>151</v>
       </c>
       <c r="B57">
-        <v>4861</v>
+        <v>5425</v>
       </c>
     </row>
     <row r="58" spans="1:2">
@@ -3555,7 +3555,7 @@
         <v>45</v>
       </c>
       <c r="B58">
-        <v>4140</v>
+        <v>4216</v>
       </c>
     </row>
     <row r="59" spans="1:2">
@@ -3563,7 +3563,7 @@
         <v>46</v>
       </c>
       <c r="B59">
-        <v>4003</v>
+        <v>4094</v>
       </c>
     </row>
     <row r="60" spans="1:2">
@@ -3571,7 +3571,7 @@
         <v>47</v>
       </c>
       <c r="B60">
-        <v>2448</v>
+        <v>2538</v>
       </c>
     </row>
     <row r="61" spans="1:2">
@@ -3579,7 +3579,7 @@
         <v>152</v>
       </c>
       <c r="B61">
-        <v>1876</v>
+        <v>2050</v>
       </c>
     </row>
     <row r="62" spans="1:2">
@@ -3587,7 +3587,7 @@
         <v>153</v>
       </c>
       <c r="B62">
-        <v>1876</v>
+        <v>2050</v>
       </c>
     </row>
     <row r="63" spans="1:2">
@@ -3595,7 +3595,7 @@
         <v>49</v>
       </c>
       <c r="B63">
-        <v>1080</v>
+        <v>1166</v>
       </c>
     </row>
     <row r="64" spans="1:2">
@@ -3640,46 +3640,46 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B2">
         <v>100</v>
       </c>
       <c r="C2">
-        <v>119</v>
+        <v>120</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B3">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="C3">
-        <v>97</v>
+        <v>100</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="1" t="s">
-        <v>23</v>
+        <v>5</v>
       </c>
       <c r="B4">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="C4">
-        <v>99</v>
+        <v>108</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" s="1" t="s">
-        <v>5</v>
+        <v>23</v>
       </c>
       <c r="B5">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="C5">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -3690,7 +3690,7 @@
         <v>58</v>
       </c>
       <c r="C6">
-        <v>64</v>
+        <v>65</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -3701,7 +3701,7 @@
         <v>58</v>
       </c>
       <c r="C7">
-        <v>64</v>
+        <v>65</v>
       </c>
     </row>
     <row r="8" spans="1:3">
@@ -3709,10 +3709,10 @@
         <v>31</v>
       </c>
       <c r="B8">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C8">
-        <v>57</v>
+        <v>59</v>
       </c>
     </row>
     <row r="9" spans="1:3">
@@ -3720,10 +3720,10 @@
         <v>15</v>
       </c>
       <c r="B9">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C9">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="10" spans="1:3">
@@ -3731,15 +3731,15 @@
         <v>18</v>
       </c>
       <c r="B10">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="C10">
-        <v>45</v>
+        <v>48</v>
       </c>
     </row>
     <row r="11" spans="1:3">
       <c r="A11" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B11">
         <v>34</v>
@@ -3778,7 +3778,7 @@
         <v>32</v>
       </c>
       <c r="C14">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="15" spans="1:3">
@@ -3827,46 +3827,46 @@
     </row>
     <row r="19" spans="1:3">
       <c r="A19" s="1" t="s">
-        <v>126</v>
+        <v>148</v>
       </c>
       <c r="B19">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="C19">
-        <v>41</v>
+        <v>28</v>
       </c>
     </row>
     <row r="20" spans="1:3">
       <c r="A20" s="1" t="s">
-        <v>127</v>
+        <v>149</v>
       </c>
       <c r="B20">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="C20">
-        <v>41</v>
+        <v>28</v>
       </c>
     </row>
     <row r="21" spans="1:3">
       <c r="A21" s="1" t="s">
-        <v>148</v>
+        <v>126</v>
       </c>
       <c r="B21">
         <v>25</v>
       </c>
       <c r="C21">
-        <v>26</v>
+        <v>42</v>
       </c>
     </row>
     <row r="22" spans="1:3">
       <c r="A22" s="1" t="s">
-        <v>149</v>
+        <v>127</v>
       </c>
       <c r="B22">
         <v>25</v>
       </c>
       <c r="C22">
-        <v>26</v>
+        <v>42</v>
       </c>
     </row>
     <row r="23" spans="1:3">
@@ -3959,13 +3959,13 @@
     </row>
     <row r="31" spans="1:3">
       <c r="A31" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B31">
         <v>12</v>
       </c>
       <c r="C31">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="32" spans="1:3">
@@ -3973,10 +3973,10 @@
         <v>145</v>
       </c>
       <c r="B32">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C32">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="33" spans="1:3">
@@ -3984,10 +3984,10 @@
         <v>146</v>
       </c>
       <c r="B33">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C33">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="34" spans="1:3">
@@ -3995,10 +3995,10 @@
         <v>147</v>
       </c>
       <c r="B34">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C34">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="35" spans="1:3">
@@ -4014,7 +4014,7 @@
     </row>
     <row r="36" spans="1:3">
       <c r="A36" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B36">
         <v>8</v>
@@ -4368,7 +4368,7 @@
         <v>4</v>
       </c>
       <c r="B2">
-        <v>138148</v>
+        <v>147082</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -4376,7 +4376,7 @@
         <v>128</v>
       </c>
       <c r="B3">
-        <v>96907</v>
+        <v>99991</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -4384,7 +4384,7 @@
         <v>129</v>
       </c>
       <c r="B4">
-        <v>96907</v>
+        <v>99991</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -4392,7 +4392,7 @@
         <v>126</v>
       </c>
       <c r="B5">
-        <v>88196</v>
+        <v>94648</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -4400,15 +4400,15 @@
         <v>127</v>
       </c>
       <c r="B6">
-        <v>88196</v>
+        <v>94648</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B7">
-        <v>84178</v>
+        <v>89181</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -4416,7 +4416,7 @@
         <v>16</v>
       </c>
       <c r="B8">
-        <v>66583</v>
+        <v>69549</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -4424,7 +4424,7 @@
         <v>22</v>
       </c>
       <c r="B9">
-        <v>58202</v>
+        <v>61960</v>
       </c>
     </row>
     <row r="10" spans="1:2">
@@ -4432,15 +4432,15 @@
         <v>5</v>
       </c>
       <c r="B10">
-        <v>45584</v>
+        <v>49556</v>
       </c>
     </row>
     <row r="11" spans="1:2">
       <c r="A11" s="1" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="B11">
-        <v>39031</v>
+        <v>36609</v>
       </c>
     </row>
     <row r="12" spans="1:2">
@@ -4448,7 +4448,7 @@
         <v>124</v>
       </c>
       <c r="B12">
-        <v>33883</v>
+        <v>35234</v>
       </c>
     </row>
     <row r="13" spans="1:2">
@@ -4456,63 +4456,63 @@
         <v>125</v>
       </c>
       <c r="B13">
-        <v>33883</v>
+        <v>35234</v>
       </c>
     </row>
     <row r="14" spans="1:2">
       <c r="A14" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B14">
-        <v>33634</v>
+        <v>29971</v>
       </c>
     </row>
     <row r="15" spans="1:2">
       <c r="A15" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B15">
-        <v>28389</v>
+        <v>22750</v>
       </c>
     </row>
     <row r="16" spans="1:2">
       <c r="A16" s="1" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="B16">
-        <v>21409</v>
+        <v>22157</v>
       </c>
     </row>
     <row r="17" spans="1:2">
       <c r="A17" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B17">
-        <v>21192</v>
+        <v>20881</v>
       </c>
     </row>
     <row r="18" spans="1:2">
       <c r="A18" s="1" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="B18">
-        <v>20019</v>
+        <v>20178</v>
       </c>
     </row>
     <row r="19" spans="1:2">
       <c r="A19" s="1" t="s">
-        <v>18</v>
+        <v>30</v>
       </c>
       <c r="B19">
-        <v>19051</v>
+        <v>18836</v>
       </c>
     </row>
     <row r="20" spans="1:2">
       <c r="A20" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B20">
-        <v>17680</v>
+        <v>17374</v>
       </c>
     </row>
     <row r="21" spans="1:2">
@@ -4520,7 +4520,7 @@
         <v>141</v>
       </c>
       <c r="B21">
-        <v>16254</v>
+        <v>17079</v>
       </c>
     </row>
     <row r="22" spans="1:2">
@@ -4528,324 +4528,324 @@
         <v>142</v>
       </c>
       <c r="B22">
-        <v>16254</v>
+        <v>17079</v>
       </c>
     </row>
     <row r="23" spans="1:2">
       <c r="A23" s="1" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B23">
-        <v>16246</v>
+        <v>16918</v>
       </c>
     </row>
     <row r="24" spans="1:2">
       <c r="A24" s="1" t="s">
-        <v>31</v>
+        <v>154</v>
       </c>
       <c r="B24">
-        <v>16165</v>
+        <v>16317</v>
       </c>
     </row>
     <row r="25" spans="1:2">
       <c r="A25" s="1" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="B25">
-        <v>15567</v>
+        <v>16317</v>
       </c>
     </row>
     <row r="26" spans="1:2">
       <c r="A26" s="1" t="s">
-        <v>155</v>
+        <v>34</v>
       </c>
       <c r="B26">
-        <v>15567</v>
+        <v>16197</v>
       </c>
     </row>
     <row r="27" spans="1:2">
       <c r="A27" s="1" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="B27">
-        <v>14908</v>
+        <v>14922</v>
       </c>
     </row>
     <row r="28" spans="1:2">
       <c r="A28" s="1" t="s">
-        <v>26</v>
+        <v>132</v>
       </c>
       <c r="B28">
-        <v>14089</v>
+        <v>13578</v>
       </c>
     </row>
     <row r="29" spans="1:2">
       <c r="A29" s="1" t="s">
-        <v>43</v>
+        <v>133</v>
       </c>
       <c r="B29">
-        <v>13100</v>
+        <v>13578</v>
       </c>
     </row>
     <row r="30" spans="1:2">
       <c r="A30" s="1" t="s">
-        <v>132</v>
+        <v>43</v>
       </c>
       <c r="B30">
-        <v>12437</v>
+        <v>13578</v>
       </c>
     </row>
     <row r="31" spans="1:2">
       <c r="A31" s="1" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="B31">
-        <v>12437</v>
+        <v>13061</v>
       </c>
     </row>
     <row r="32" spans="1:2">
       <c r="A32" s="1" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="B32">
-        <v>12187</v>
+        <v>13061</v>
       </c>
     </row>
     <row r="33" spans="1:2">
       <c r="A33" s="1" t="s">
-        <v>131</v>
+        <v>24</v>
       </c>
       <c r="B33">
-        <v>12187</v>
+        <v>11527</v>
       </c>
     </row>
     <row r="34" spans="1:2">
       <c r="A34" s="1" t="s">
-        <v>24</v>
+        <v>134</v>
       </c>
       <c r="B34">
-        <v>10989</v>
+        <v>10788</v>
       </c>
     </row>
     <row r="35" spans="1:2">
       <c r="A35" s="1" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="B35">
-        <v>10335</v>
+        <v>10788</v>
       </c>
     </row>
     <row r="36" spans="1:2">
       <c r="A36" s="1" t="s">
-        <v>135</v>
+        <v>17</v>
       </c>
       <c r="B36">
-        <v>10335</v>
+        <v>10398</v>
       </c>
     </row>
     <row r="37" spans="1:2">
       <c r="A37" s="1" t="s">
-        <v>17</v>
+        <v>36</v>
       </c>
       <c r="B37">
-        <v>10032</v>
+        <v>9833</v>
       </c>
     </row>
     <row r="38" spans="1:2">
       <c r="A38" s="1" t="s">
-        <v>35</v>
+        <v>136</v>
       </c>
       <c r="B38">
-        <v>9391</v>
+        <v>8691</v>
       </c>
     </row>
     <row r="39" spans="1:2">
       <c r="A39" s="1" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
       <c r="B39">
-        <v>9013</v>
+        <v>8691</v>
       </c>
     </row>
     <row r="40" spans="1:2">
       <c r="A40" s="1" t="s">
-        <v>144</v>
+        <v>35</v>
       </c>
       <c r="B40">
-        <v>9013</v>
+        <v>8528</v>
       </c>
     </row>
     <row r="41" spans="1:2">
       <c r="A41" s="1" t="s">
-        <v>136</v>
+        <v>47</v>
       </c>
       <c r="B41">
-        <v>8297</v>
+        <v>8088</v>
       </c>
     </row>
     <row r="42" spans="1:2">
       <c r="A42" s="1" t="s">
-        <v>137</v>
+        <v>150</v>
       </c>
       <c r="B42">
-        <v>8297</v>
+        <v>7162</v>
       </c>
     </row>
     <row r="43" spans="1:2">
       <c r="A43" s="1" t="s">
-        <v>36</v>
+        <v>151</v>
       </c>
       <c r="B43">
-        <v>7750</v>
+        <v>7162</v>
       </c>
     </row>
     <row r="44" spans="1:2">
       <c r="A44" s="1" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="B44">
-        <v>7591</v>
+        <v>7056</v>
       </c>
     </row>
     <row r="45" spans="1:2">
       <c r="A45" s="1" t="s">
-        <v>40</v>
+        <v>138</v>
       </c>
       <c r="B45">
-        <v>6876</v>
+        <v>6899</v>
       </c>
     </row>
     <row r="46" spans="1:2">
       <c r="A46" s="1" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="B46">
-        <v>6627</v>
+        <v>6899</v>
       </c>
     </row>
     <row r="47" spans="1:2">
       <c r="A47" s="1" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="B47">
-        <v>6627</v>
+        <v>6899</v>
       </c>
     </row>
     <row r="48" spans="1:2">
       <c r="A48" s="1" t="s">
-        <v>140</v>
+        <v>49</v>
       </c>
       <c r="B48">
-        <v>6627</v>
+        <v>5109</v>
       </c>
     </row>
     <row r="49" spans="1:2">
       <c r="A49" s="1" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="B49">
-        <v>6334</v>
+        <v>4157</v>
       </c>
     </row>
     <row r="50" spans="1:2">
       <c r="A50" s="1" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
       <c r="B50">
-        <v>6334</v>
+        <v>4157</v>
       </c>
     </row>
     <row r="51" spans="1:2">
       <c r="A51" s="1" t="s">
-        <v>49</v>
+        <v>147</v>
       </c>
       <c r="B51">
-        <v>4933</v>
+        <v>4157</v>
       </c>
     </row>
     <row r="52" spans="1:2">
       <c r="A52" s="1" t="s">
-        <v>145</v>
+        <v>46</v>
       </c>
       <c r="B52">
-        <v>4045</v>
+        <v>2165</v>
       </c>
     </row>
     <row r="53" spans="1:2">
       <c r="A53" s="1" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="B53">
-        <v>4045</v>
+        <v>1502</v>
       </c>
     </row>
     <row r="54" spans="1:2">
       <c r="A54" s="1" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="B54">
-        <v>4045</v>
+        <v>1502</v>
       </c>
     </row>
     <row r="55" spans="1:2">
       <c r="A55" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B55">
-        <v>2086</v>
+        <v>1472</v>
       </c>
     </row>
     <row r="56" spans="1:2">
       <c r="A56" s="1" t="s">
-        <v>148</v>
+        <v>42</v>
       </c>
       <c r="B56">
-        <v>1457</v>
+        <v>1376</v>
       </c>
     </row>
     <row r="57" spans="1:2">
       <c r="A57" s="1" t="s">
-        <v>149</v>
+        <v>152</v>
       </c>
       <c r="B57">
-        <v>1457</v>
+        <v>503</v>
       </c>
     </row>
     <row r="58" spans="1:2">
       <c r="A58" s="1" t="s">
-        <v>45</v>
+        <v>153</v>
       </c>
       <c r="B58">
-        <v>1419</v>
+        <v>503</v>
       </c>
     </row>
     <row r="59" spans="1:2">
       <c r="A59" s="1" t="s">
-        <v>42</v>
+        <v>143</v>
       </c>
       <c r="B59">
-        <v>1274</v>
+        <v>0</v>
       </c>
     </row>
     <row r="60" spans="1:2">
       <c r="A60" s="1" t="s">
-        <v>152</v>
+        <v>20</v>
       </c>
       <c r="B60">
-        <v>459</v>
+        <v>0</v>
       </c>
     </row>
     <row r="61" spans="1:2">
       <c r="A61" s="1" t="s">
-        <v>153</v>
+        <v>7</v>
       </c>
       <c r="B61">
-        <v>459</v>
+        <v>0</v>
       </c>
     </row>
     <row r="62" spans="1:2">
       <c r="A62" s="1" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="B62">
         <v>0</v>
@@ -4853,7 +4853,7 @@
     </row>
     <row r="63" spans="1:2">
       <c r="A63" s="1" t="s">
-        <v>9</v>
+        <v>23</v>
       </c>
       <c r="B63">
         <v>0</v>
@@ -4861,7 +4861,7 @@
     </row>
     <row r="64" spans="1:2">
       <c r="A64" s="1" t="s">
-        <v>23</v>
+        <v>144</v>
       </c>
       <c r="B64">
         <v>0</v>
@@ -4901,7 +4901,7 @@
         <v>97</v>
       </c>
       <c r="B2">
-        <v>2443226</v>
+        <v>2631252</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -4909,7 +4909,7 @@
         <v>99</v>
       </c>
       <c r="B3">
-        <v>2133662</v>
+        <v>2176221</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -4917,7 +4917,7 @@
         <v>156</v>
       </c>
       <c r="B4">
-        <v>1215313</v>
+        <v>1296610</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -4925,7 +4925,7 @@
         <v>157</v>
       </c>
       <c r="B5">
-        <v>1215313</v>
+        <v>1296610</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -4933,23 +4933,23 @@
         <v>101</v>
       </c>
       <c r="B6">
-        <v>978011</v>
+        <v>1018354</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" s="1" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="B7">
-        <v>818990</v>
+        <v>847393</v>
       </c>
     </row>
     <row r="8" spans="1:2">
       <c r="A8" s="1" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B8">
-        <v>794328</v>
+        <v>830548</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -4957,7 +4957,7 @@
         <v>107</v>
       </c>
       <c r="B9">
-        <v>557928</v>
+        <v>579433</v>
       </c>
     </row>
     <row r="10" spans="1:2">
@@ -4965,7 +4965,7 @@
         <v>158</v>
       </c>
       <c r="B10">
-        <v>365179</v>
+        <v>473116</v>
       </c>
     </row>
     <row r="11" spans="1:2">
@@ -4973,7 +4973,7 @@
         <v>159</v>
       </c>
       <c r="B11">
-        <v>365179</v>
+        <v>473116</v>
       </c>
     </row>
     <row r="12" spans="1:2">
@@ -4981,7 +4981,7 @@
         <v>105</v>
       </c>
       <c r="B12">
-        <v>311782</v>
+        <v>336188</v>
       </c>
     </row>
     <row r="13" spans="1:2">
@@ -4989,7 +4989,7 @@
         <v>106</v>
       </c>
       <c r="B13">
-        <v>284844</v>
+        <v>303531</v>
       </c>
     </row>
     <row r="14" spans="1:2">
@@ -4997,7 +4997,7 @@
         <v>110</v>
       </c>
       <c r="B14">
-        <v>182431</v>
+        <v>189848</v>
       </c>
     </row>
     <row r="15" spans="1:2">
@@ -5005,7 +5005,7 @@
         <v>160</v>
       </c>
       <c r="B15">
-        <v>169834</v>
+        <v>179542</v>
       </c>
     </row>
     <row r="16" spans="1:2">
@@ -5013,7 +5013,7 @@
         <v>161</v>
       </c>
       <c r="B16">
-        <v>77822</v>
+        <v>78952</v>
       </c>
     </row>
     <row r="17" spans="1:2">
@@ -5021,7 +5021,7 @@
         <v>162</v>
       </c>
       <c r="B17">
-        <v>77822</v>
+        <v>78952</v>
       </c>
     </row>
     <row r="18" spans="1:2">
@@ -5029,7 +5029,7 @@
         <v>111</v>
       </c>
       <c r="B18">
-        <v>50732</v>
+        <v>53227</v>
       </c>
     </row>
     <row r="19" spans="1:2">
@@ -5037,7 +5037,7 @@
         <v>117</v>
       </c>
       <c r="B19">
-        <v>14501</v>
+        <v>14840</v>
       </c>
     </row>
     <row r="20" spans="1:2">
@@ -5045,7 +5045,7 @@
         <v>163</v>
       </c>
       <c r="B20">
-        <v>10201</v>
+        <v>10488</v>
       </c>
     </row>
     <row r="21" spans="1:2">
@@ -5053,7 +5053,7 @@
         <v>112</v>
       </c>
       <c r="B21">
-        <v>8549</v>
+        <v>8751</v>
       </c>
     </row>
     <row r="22" spans="1:2">
@@ -5061,7 +5061,7 @@
         <v>164</v>
       </c>
       <c r="B22">
-        <v>6358</v>
+        <v>6530</v>
       </c>
     </row>
     <row r="23" spans="1:2">
@@ -5069,7 +5069,7 @@
         <v>165</v>
       </c>
       <c r="B23">
-        <v>5923</v>
+        <v>6045</v>
       </c>
     </row>
     <row r="24" spans="1:2">
@@ -5077,7 +5077,7 @@
         <v>166</v>
       </c>
       <c r="B24">
-        <v>5923</v>
+        <v>6045</v>
       </c>
     </row>
     <row r="25" spans="1:2">
@@ -5085,7 +5085,7 @@
         <v>116</v>
       </c>
       <c r="B25">
-        <v>4861</v>
+        <v>5425</v>
       </c>
     </row>
     <row r="26" spans="1:2">
@@ -5093,7 +5093,7 @@
         <v>118</v>
       </c>
       <c r="B26">
-        <v>1876</v>
+        <v>2050</v>
       </c>
     </row>
     <row r="27" spans="1:2">
@@ -5101,7 +5101,7 @@
         <v>167</v>
       </c>
       <c r="B27">
-        <v>1080</v>
+        <v>1166</v>
       </c>
     </row>
     <row r="28" spans="1:2">
@@ -5149,10 +5149,10 @@
         <v>107</v>
       </c>
       <c r="B2">
-        <v>345</v>
+        <v>353</v>
       </c>
       <c r="C2">
-        <v>391</v>
+        <v>402</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -5160,10 +5160,10 @@
         <v>101</v>
       </c>
       <c r="B3">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="C3">
-        <v>258</v>
+        <v>261</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -5171,10 +5171,10 @@
         <v>110</v>
       </c>
       <c r="B4">
-        <v>166</v>
+        <v>169</v>
       </c>
       <c r="C4">
-        <v>204</v>
+        <v>208</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -5182,10 +5182,10 @@
         <v>156</v>
       </c>
       <c r="B5">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="C5">
-        <v>103</v>
+        <v>108</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -5193,10 +5193,10 @@
         <v>157</v>
       </c>
       <c r="B6">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="C6">
-        <v>103</v>
+        <v>108</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -5204,10 +5204,10 @@
         <v>163</v>
       </c>
       <c r="B7">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="C7">
-        <v>62</v>
+        <v>65</v>
       </c>
     </row>
     <row r="8" spans="1:3">
@@ -5223,13 +5223,13 @@
     </row>
     <row r="9" spans="1:3">
       <c r="A9" s="1" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="B9">
         <v>26</v>
       </c>
       <c r="C9">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="10" spans="1:3">
@@ -5240,7 +5240,7 @@
         <v>25</v>
       </c>
       <c r="C10">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="11" spans="1:3">
@@ -5475,10 +5475,10 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2" s="1" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="B2">
-        <v>305870</v>
+        <v>320681</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -5486,71 +5486,71 @@
         <v>97</v>
       </c>
       <c r="B3">
-        <v>138148</v>
+        <v>147082</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" s="1" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
       <c r="B4">
-        <v>91548</v>
+        <v>94648</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" s="1" t="s">
-        <v>100</v>
+        <v>107</v>
       </c>
       <c r="B5">
-        <v>88196</v>
+        <v>88452</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" s="1" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="B6">
-        <v>72914</v>
+        <v>73359</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" s="1" t="s">
-        <v>101</v>
+        <v>110</v>
       </c>
       <c r="B7">
-        <v>69514</v>
+        <v>59477</v>
       </c>
     </row>
     <row r="8" spans="1:2">
       <c r="A8" s="1" t="s">
-        <v>110</v>
+        <v>156</v>
       </c>
       <c r="B8">
-        <v>56458</v>
+        <v>49556</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="A9" s="1" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="B9">
-        <v>45584</v>
+        <v>49556</v>
       </c>
     </row>
     <row r="10" spans="1:2">
       <c r="A10" s="1" t="s">
-        <v>157</v>
+        <v>105</v>
       </c>
       <c r="B10">
-        <v>45584</v>
+        <v>36609</v>
       </c>
     </row>
     <row r="11" spans="1:2">
       <c r="A11" s="1" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="B11">
-        <v>33634</v>
+        <v>35234</v>
       </c>
     </row>
     <row r="12" spans="1:2">
@@ -5558,7 +5558,7 @@
         <v>106</v>
       </c>
       <c r="B12">
-        <v>21409</v>
+        <v>22750</v>
       </c>
     </row>
     <row r="13" spans="1:2">
@@ -5566,7 +5566,7 @@
         <v>158</v>
       </c>
       <c r="B13">
-        <v>21192</v>
+        <v>22157</v>
       </c>
     </row>
     <row r="14" spans="1:2">
@@ -5574,7 +5574,7 @@
         <v>159</v>
       </c>
       <c r="B14">
-        <v>21192</v>
+        <v>22157</v>
       </c>
     </row>
     <row r="15" spans="1:2">
@@ -5582,7 +5582,7 @@
         <v>160</v>
       </c>
       <c r="B15">
-        <v>19423</v>
+        <v>20231</v>
       </c>
     </row>
     <row r="16" spans="1:2">
@@ -5590,7 +5590,7 @@
         <v>168</v>
       </c>
       <c r="B16">
-        <v>15567</v>
+        <v>16317</v>
       </c>
     </row>
     <row r="17" spans="1:2">
@@ -5598,7 +5598,7 @@
         <v>169</v>
       </c>
       <c r="B17">
-        <v>15567</v>
+        <v>16317</v>
       </c>
     </row>
     <row r="18" spans="1:2">
@@ -5606,7 +5606,7 @@
         <v>111</v>
       </c>
       <c r="B18">
-        <v>15268</v>
+        <v>15897</v>
       </c>
     </row>
     <row r="19" spans="1:2">
@@ -5614,7 +5614,7 @@
         <v>165</v>
       </c>
       <c r="B19">
-        <v>13100</v>
+        <v>13578</v>
       </c>
     </row>
     <row r="20" spans="1:2">
@@ -5622,7 +5622,7 @@
         <v>166</v>
       </c>
       <c r="B20">
-        <v>13100</v>
+        <v>13578</v>
       </c>
     </row>
     <row r="21" spans="1:2">
@@ -5630,7 +5630,7 @@
         <v>161</v>
       </c>
       <c r="B21">
-        <v>10989</v>
+        <v>11527</v>
       </c>
     </row>
     <row r="22" spans="1:2">
@@ -5638,7 +5638,7 @@
         <v>162</v>
       </c>
       <c r="B22">
-        <v>10989</v>
+        <v>11527</v>
       </c>
     </row>
     <row r="23" spans="1:2">
@@ -5646,23 +5646,23 @@
         <v>163</v>
       </c>
       <c r="B23">
-        <v>9048</v>
+        <v>9590</v>
       </c>
     </row>
     <row r="24" spans="1:2">
       <c r="A24" s="1" t="s">
-        <v>112</v>
+        <v>116</v>
       </c>
       <c r="B24">
-        <v>6876</v>
+        <v>7162</v>
       </c>
     </row>
     <row r="25" spans="1:2">
       <c r="A25" s="1" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="B25">
-        <v>6334</v>
+        <v>7056</v>
       </c>
     </row>
     <row r="26" spans="1:2">
@@ -5670,7 +5670,7 @@
         <v>167</v>
       </c>
       <c r="B26">
-        <v>4933</v>
+        <v>5109</v>
       </c>
     </row>
     <row r="27" spans="1:2">
@@ -5678,7 +5678,7 @@
         <v>117</v>
       </c>
       <c r="B27">
-        <v>4779</v>
+        <v>5013</v>
       </c>
     </row>
     <row r="28" spans="1:2">
@@ -5686,7 +5686,7 @@
         <v>164</v>
       </c>
       <c r="B28">
-        <v>1274</v>
+        <v>1376</v>
       </c>
     </row>
     <row r="29" spans="1:2">
@@ -5694,7 +5694,7 @@
         <v>118</v>
       </c>
       <c r="B29">
-        <v>459</v>
+        <v>503</v>
       </c>
     </row>
   </sheetData>

</xml_diff>